<commit_message>
Test case authoring in progress
</commit_message>
<xml_diff>
--- a/SwagLabs Manual Test Cases/SwagLabsTests.xlsx
+++ b/SwagLabs Manual Test Cases/SwagLabsTests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Manual-Test-Cases\SwagLabs Manual Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DD634E-6037-44C4-ACF9-B3D6770DD98F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B8253A-4614-44A8-B07D-EBFFA5753F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="722" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="722" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -112,13 +112,109 @@
   </si>
   <si>
     <t>LP002</t>
+  </si>
+  <si>
+    <t>1. Open any browser and navigate to https://www.saucedemo.com.</t>
+  </si>
+  <si>
+    <t>2. Enter locked_out_user in the UserName field.</t>
+  </si>
+  <si>
+    <t>userName: locked_out_user</t>
+  </si>
+  <si>
+    <t>Login with locked out user name and valid password</t>
+  </si>
+  <si>
+    <t>User cannot log in.
+Error message appears : Epic sadface: Sorry, this user has been locked out.</t>
+  </si>
+  <si>
+    <t>4. Click on the Login button.</t>
+  </si>
+  <si>
+    <t>3. Enter wrong password in the Password field.</t>
+  </si>
+  <si>
+    <t>password: wrongPass</t>
+  </si>
+  <si>
+    <t>User cannot log in.
+Epic sadface: Username and password do not match any user in this service.</t>
+  </si>
+  <si>
+    <t>LP003</t>
+  </si>
+  <si>
+    <t>2. Leave UserName field empty.</t>
+  </si>
+  <si>
+    <t>3. Leave Password field empty.</t>
+  </si>
+  <si>
+    <t>Try to login with valid user name and wrong password and check the error message</t>
+  </si>
+  <si>
+    <t>User cannot log in.
+Epic sadface: Username is required.</t>
+  </si>
+  <si>
+    <t>userName: empty</t>
+  </si>
+  <si>
+    <t>Try to log in with empty user name and valid password to check the error messages.</t>
+  </si>
+  <si>
+    <t>Try to log in with valid user name and empty password to check the error messages.</t>
+  </si>
+  <si>
+    <t>password: empty</t>
+  </si>
+  <si>
+    <t>LP004</t>
+  </si>
+  <si>
+    <t>LP005</t>
+  </si>
+  <si>
+    <t>Automate</t>
+  </si>
+  <si>
+    <t>User logged in and redirected to Products Page</t>
+  </si>
+  <si>
+    <t>Check the Products Page Information and layout.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On the Products page check the following:
+1. Title "Products" is displayed.
+2. There are products available on the Products page.
+3. There is a shopping cart icon displayed in the upper left corner on the page.
+4. There is a filter icon and dropdown menu displayed in the upper left corner on the page. </t>
+  </si>
+  <si>
+    <t>All expected information, products, menus are displayed in their appropriate places.</t>
+  </si>
+  <si>
+    <t>Check the Products Information and layout.</t>
+  </si>
+  <si>
+    <t>For each displayed product check the following:
+1. The product has title.
+2.  The product has image.
+3. The product has description.
+4. The product has price. 
+5. The product has Ass to Cart button.</t>
+  </si>
+  <si>
+    <t>All expected information is displayed.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +254,12 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -272,7 +374,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -281,6 +383,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -290,9 +395,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -301,6 +403,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -667,17 +778,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07E5368-0831-4ADD-BA76-A58B0877635A}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
     <col min="4" max="4" width="49" customWidth="1"/>
     <col min="5" max="6" width="28.85546875" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
@@ -711,17 +822,17 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>18</v>
+      <c r="D2" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>25</v>
@@ -729,13 +840,15 @@
       <c r="F2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
@@ -743,160 +856,297 @@
       <c r="F3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="9"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
       <c r="D5" s="3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E5" s="10"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="9"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E9" s="10"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="C10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E12" s="9"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E13" s="10"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="G10:G13"/>
+  <mergeCells count="35">
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F16:F17"/>
     <mergeCell ref="H10:H13"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="H2:H5"/>
@@ -913,21 +1163,193 @@
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G2:G5"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="G10:G13"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F0869F6-BEF5-405D-A4B5-E151EBA21016}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="49" customWidth="1"/>
+    <col min="5" max="6" width="28.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="F4:F5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Test case authoring for products page section is in progress
</commit_message>
<xml_diff>
--- a/SwagLabs Manual Test Cases/SwagLabsTests.xlsx
+++ b/SwagLabs Manual Test Cases/SwagLabsTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Manual-Test-Cases\SwagLabs Manual Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B8253A-4614-44A8-B07D-EBFFA5753F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39529B01-20A8-4B5B-AD68-BD0E22EED268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="722" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="62">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -208,6 +208,28 @@
   </si>
   <si>
     <t>All expected information is displayed.</t>
+  </si>
+  <si>
+    <t>Add product to the shopping cart</t>
+  </si>
+  <si>
+    <t>1. On the Products page click on the Add to Cart buton to add a product to the shopping cart.</t>
+  </si>
+  <si>
+    <t>The Add to Cart button changes to Remove button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product is added to the shopping cart.
+</t>
+  </si>
+  <si>
+    <t>A red badge, displaying the numbers of products in the cart appears above the shopping cart icon.</t>
+  </si>
+  <si>
+    <t>Remove product from the shopping cart</t>
+  </si>
+  <si>
+    <t>1. On the Products page click on theRemove buton to remove a product from the shopping cart.</t>
   </si>
 </sst>
 </file>
@@ -374,7 +396,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -412,6 +434,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1133,20 +1171,11 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="G10:G13"/>
     <mergeCell ref="H10:H13"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="H2:H5"/>
@@ -1163,11 +1192,20 @@
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G2:G5"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F16:F17"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1176,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F0869F6-BEF5-405D-A4B5-E151EBA21016}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,7 +1226,8 @@
     <col min="2" max="2" width="29.85546875" customWidth="1"/>
     <col min="3" max="3" width="45.7109375" customWidth="1"/>
     <col min="4" max="4" width="49" customWidth="1"/>
-    <col min="5" max="6" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="49.140625" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" customWidth="1"/>
   </cols>
@@ -1288,7 +1327,7 @@
       <c r="D6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="5" t="s">
         <v>54</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -1304,7 +1343,7 @@
       <c r="B7" s="9"/>
       <c r="C7" s="6"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="9"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="3" t="s">
         <v>22</v>
       </c>
@@ -1316,7 +1355,7 @@
       <c r="B8" s="9"/>
       <c r="C8" s="6"/>
       <c r="D8" s="12"/>
-      <c r="E8" s="9"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="5"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -1326,13 +1365,147 @@
       <c r="B9" s="10"/>
       <c r="C9" s="7"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="10"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
+    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="30">
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
     <mergeCell ref="H6:H9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="D2:D5"/>

</xml_diff>

<commit_message>
E2E test cases in progress
</commit_message>
<xml_diff>
--- a/SwagLabs Manual Test Cases/SwagLabsTests.xlsx
+++ b/SwagLabs Manual Test Cases/SwagLabsTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Manual-Test-Cases\SwagLabs Manual Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D8C4C1-6F41-404E-A693-9EC6EE5AE65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4175E882-CB4F-46AB-B4EE-F7546F927527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="836" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="169">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -583,6 +583,62 @@
   </si>
   <si>
     <t>E2E008</t>
+  </si>
+  <si>
+    <t>Purchase all products.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Log in the AUT with valid username and password.
+2. Navigate to the products page and add all products to the shopping cart.
+3. Click on the shopping cart icon and reach the Shopping cart page.
+4. Click on the Continue button and navigate the Checkout page.
+5. In the checkout page populate all required fields with valid data and click the Continue button.
+6. In the checkout Overview Page check if the pricess are calculated correctly.
+7. Click on the Finish button and navigate to the Checkout Complete Page.
+8. Verify that the text "Thank you for your order!" is displayed.
+9. Click on the Back Home button.
+10. Verify that the user is redirected to the Products page in the AUT.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchase the first 2 products when products are sorted by Name(Z to A) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Log in the AUT with valid username and password.
+2. Navigate to the products page and click on the sort drop down menu. 
+3. Select Name(Z to A).
+4. Add the first 2 products to the shopping cart.
+5. Click on the shopping cart icon and reach the Shopping cart page.
+6. Click on the Continue button and navigate the Checkout page.
+7. In the checkout page populate all required fields with valid data and click the Continue button.
+8. In the checkout Overview Page check if the pricess are calculated correctly.
+9. Click on the Finish button and navigate to the Checkout Complete Page.
+10. Verify that the text "Thank you for your order!" is displayed.
+11. Click on the Back Home button.
+12. Verify that the user is redirected to the Products page in the AUT.
+</t>
+  </si>
+  <si>
+    <t>Purchase the first product when products are sorted by Price(Low to High) and the first 2 products when products are sorted by Price(High to Low)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Log in the AUT with valid username and password.
+2. Navigate to the products page and click on the sort drop down menu. 
+3. Select Price (Low to High).
+4. Add the first 2 products to the shopping cart.
+5. Click on the shopping cart icon and reach the Shopping cart page.
+6. Remove the second product from the shopping cart.
+7. Click on Continue Shopping button.
+8. In Products Page click on the sort dropdown menu and select Price(High to Low).
+9. Add the first product to the shopping cart.
+10. Navigate to the shopping cart and click on the Checkout button.
+11. In the checkout page populate all required fields with valid data and click the Continue button.
+12. In the checkout Overview Page check if the pricess are calculated correctly.
+13. Click on the Finish button and navigate to the Checkout Complete Page.
+14. Verify that the text "Thank you for your order!" is displayed.
+15. Click on the Back Home button.
+16. Verify that the user is redirected to the Products page in the AUT.
+</t>
   </si>
 </sst>
 </file>
@@ -1523,11 +1579,20 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F16:F17"/>
     <mergeCell ref="H10:H13"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="H2:H5"/>
@@ -1544,20 +1609,11 @@
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G2:G5"/>
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="G10:G13"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2130,20 +2186,41 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="F19:F21"/>
     <mergeCell ref="H6:H9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="D2:D5"/>
@@ -2160,41 +2237,20 @@
     <mergeCell ref="G2:G5"/>
     <mergeCell ref="H2:H5"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2671,14 +2727,49 @@
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
     <mergeCell ref="G6:G9"/>
     <mergeCell ref="H6:H9"/>
     <mergeCell ref="A10:A13"/>
@@ -2693,51 +2784,16 @@
     <mergeCell ref="C6:C9"/>
     <mergeCell ref="D6:D9"/>
     <mergeCell ref="E6:E9"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="F31:F33"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="E10:E13"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="G2:G5"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3224,30 +3280,35 @@
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="G26:G29"/>
     <mergeCell ref="H18:H21"/>
     <mergeCell ref="E18:E21"/>
     <mergeCell ref="F18:F21"/>
@@ -3264,35 +3325,30 @@
     <mergeCell ref="C18:C21"/>
     <mergeCell ref="D18:D21"/>
     <mergeCell ref="G18:G21"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="F22:F25"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G10:G13"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3741,21 +3797,48 @@
     </row>
   </sheetData>
   <mergeCells count="66">
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="G18:G21"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="C2:C5"/>
@@ -3764,7 +3847,1008 @@
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="D10:D13"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="F8:F9"/>
     <mergeCell ref="G10:G13"/>
+  </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2319F37F-1972-492D-B02D-DC879C63150C}">
+  <dimension ref="A1:H37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="49" customWidth="1"/>
+    <col min="5" max="5" width="49.140625" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="65">
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="E2:E5"/>
+  </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F76DF67-2F70-4CFF-82C4-2F7D4C565685}">
+  <dimension ref="A1:H37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="49" customWidth="1"/>
+    <col min="5" max="5" width="49.140625" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" ht="260.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="65">
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="F11:F13"/>
     <mergeCell ref="H18:H21"/>
     <mergeCell ref="F19:F21"/>
     <mergeCell ref="A14:A17"/>
@@ -3811,1016 +4895,4 @@
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2319F37F-1972-492D-B02D-DC879C63150C}">
-  <dimension ref="A1:H37"/>
-  <sheetViews>
-    <sheetView topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="E2" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" customWidth="1"/>
-    <col min="4" max="4" width="49" customWidth="1"/>
-    <col min="5" max="5" width="49.140625" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-    </row>
-  </sheetData>
-  <mergeCells count="65">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C13"/>
-  </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F76DF67-2F70-4CFF-82C4-2F7D4C565685}">
-  <dimension ref="A1:H37"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" customWidth="1"/>
-    <col min="4" max="4" width="49" customWidth="1"/>
-    <col min="5" max="5" width="49.140625" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-    </row>
-  </sheetData>
-  <mergeCells count="65">
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="G2:G5"/>
-  </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
E2E test cases written
</commit_message>
<xml_diff>
--- a/SwagLabs Manual Test Cases/SwagLabsTests.xlsx
+++ b/SwagLabs Manual Test Cases/SwagLabsTests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Manual-Test-Cases\SwagLabs Manual Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4175E882-CB4F-46AB-B4EE-F7546F927527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F3D01B-466F-4386-A4D4-7B4BB6401CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="836" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="164">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -570,28 +570,13 @@
     <t>E2E003</t>
   </si>
   <si>
-    <t>E2E004</t>
-  </si>
-  <si>
-    <t>E2E005</t>
-  </si>
-  <si>
-    <t>E2E006</t>
-  </si>
-  <si>
-    <t>E2E007</t>
-  </si>
-  <si>
-    <t>E2E008</t>
-  </si>
-  <si>
-    <t>Purchase all products.</t>
+    <t>Purchase all products and check Order</t>
   </si>
   <si>
     <t xml:space="preserve">1. Log in the AUT with valid username and password.
-2. Navigate to the products page and add all products to the shopping cart.
+2. Navigate to the products page and add all products in the shopping cart.
 3. Click on the shopping cart icon and reach the Shopping cart page.
-4. Click on the Continue button and navigate the Checkout page.
+4. Navigate to the shopping cart and click on the Checkout button.
 5. In the checkout page populate all required fields with valid data and click the Continue button.
 6. In the checkout Overview Page check if the pricess are calculated correctly.
 7. Click on the Finish button and navigate to the Checkout Complete Page.
@@ -601,43 +586,41 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Purchase the first 2 products when products are sorted by Name(Z to A) </t>
+    <t>Perform multiple product filters and purchase multiple products.</t>
   </si>
   <si>
     <t xml:space="preserve">1. Log in the AUT with valid username and password.
-2. Navigate to the products page and click on the sort drop down menu. 
-3. Select Name(Z to A).
-4. Add the first 2 products to the shopping cart.
-5. Click on the shopping cart icon and reach the Shopping cart page.
-6. Click on the Continue button and navigate the Checkout page.
-7. In the checkout page populate all required fields with valid data and click the Continue button.
-8. In the checkout Overview Page check if the pricess are calculated correctly.
-9. Click on the Finish button and navigate to the Checkout Complete Page.
-10. Verify that the text "Thank you for your order!" is displayed.
-11. Click on the Back Home button.
-12. Verify that the user is redirected to the Products page in the AUT.
+2. Navigate to the products page and sort products from Z to A.
+3. Add the first product to the shopping cart.
+add all products in the shopping cart.
+4. Click on the filter menu and sort products by price High to Low.
+5. Add the product at index 3.
+6. Click on the shopping cart icon and reach the Shopping cart page.
+7.In the shopping cart page click on Continue Shopping button.
+8. On the products page add the last product in the shopping cart and navigate back to the shopping cart.
+9. 
+In the checkout page populate all required fields with valid data and click the Continue button.
+10.On the checkout Information page fill in First Name, Last Name and Zip/PostalCode.
+11. Click on Continue button.
+12. On the checkout Overview click on the Finish button and navigate to the Checkout Complete Page.
+13. Verify that the text "Thank you for your order!" is displayed.
 </t>
   </si>
   <si>
-    <t>Purchase the first product when products are sorted by Price(Low to High) and the first 2 products when products are sorted by Price(High to Low)</t>
+    <t>Purchase multiple products and remove products from cart</t>
   </si>
   <si>
     <t xml:space="preserve">1. Log in the AUT with valid username and password.
-2. Navigate to the products page and click on the sort drop down menu. 
-3. Select Price (Low to High).
-4. Add the first 2 products to the shopping cart.
-5. Click on the shopping cart icon and reach the Shopping cart page.
-6. Remove the second product from the shopping cart.
-7. Click on Continue Shopping button.
-8. In Products Page click on the sort dropdown menu and select Price(High to Low).
-9. Add the first product to the shopping cart.
-10. Navigate to the shopping cart and click on the Checkout button.
-11. In the checkout page populate all required fields with valid data and click the Continue button.
-12. In the checkout Overview Page check if the pricess are calculated correctly.
-13. Click on the Finish button and navigate to the Checkout Complete Page.
-14. Verify that the text "Thank you for your order!" is displayed.
-15. Click on the Back Home button.
-16. Verify that the user is redirected to the Products page in the AUT.
+2. Navigate to the products page and add all products to the shopping cart.
+3. Click on the shopping cart icon and reach the Shopping cart page.
+4.In the shopping cart remove the first and the last products.
+5. Remove a product by valid index.
+6. Click on the Checkout button,
+.7. On the checkout page populate all required fields with valid data and click the Continue button.
+9.On the checkout Information page fill in First Name, Last Name and Zip/PostalCode.
+10. Click on Continue button.
+11. On the checkout Overview click on the Finish button and navigate to the Checkout Complete Page.
+12. Verify that the text "Thank you for your order!" is displayed.
 </t>
   </si>
 </sst>
@@ -805,7 +788,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -858,6 +841,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1579,20 +1571,11 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="G10:G13"/>
     <mergeCell ref="H10:H13"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="H2:H5"/>
@@ -1609,11 +1592,20 @@
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G2:G5"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F16:F17"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2186,41 +2178,20 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
     <mergeCell ref="H6:H9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="D2:D5"/>
@@ -2237,20 +2208,41 @@
     <mergeCell ref="G2:G5"/>
     <mergeCell ref="H2:H5"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="G34:G37"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2727,49 +2719,14 @@
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="G2:G5"/>
     <mergeCell ref="G6:G9"/>
     <mergeCell ref="H6:H9"/>
     <mergeCell ref="A10:A13"/>
@@ -2786,14 +2743,49 @@
     <mergeCell ref="E6:E9"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="E10:E13"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D37"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3280,35 +3272,30 @@
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="F22:F25"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
     <mergeCell ref="H18:H21"/>
     <mergeCell ref="E18:E21"/>
     <mergeCell ref="F18:F21"/>
@@ -3325,30 +3312,35 @@
     <mergeCell ref="C18:C21"/>
     <mergeCell ref="D18:D21"/>
     <mergeCell ref="G18:G21"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="G34:G37"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3797,48 +3789,18 @@
     </row>
   </sheetData>
   <mergeCells count="66">
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G10:G13"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="C2:C5"/>
@@ -3851,1004 +3813,6 @@
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="C6:C9"/>
     <mergeCell ref="D6:D9"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G10:G13"/>
-  </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2319F37F-1972-492D-B02D-DC879C63150C}">
-  <dimension ref="A1:H37"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" customWidth="1"/>
-    <col min="4" max="4" width="49" customWidth="1"/>
-    <col min="5" max="5" width="49.140625" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-    </row>
-  </sheetData>
-  <mergeCells count="65">
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="E2:E5"/>
-  </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F76DF67-2F70-4CFF-82C4-2F7D4C565685}">
-  <dimension ref="A1:H37"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" customWidth="1"/>
-    <col min="4" max="4" width="49" customWidth="1"/>
-    <col min="5" max="5" width="49.140625" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" ht="260.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-    </row>
-  </sheetData>
-  <mergeCells count="65">
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="F11:F13"/>
     <mergeCell ref="H18:H21"/>
     <mergeCell ref="F19:F21"/>
     <mergeCell ref="A14:A17"/>
@@ -4895,4 +3859,918 @@
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2319F37F-1972-492D-B02D-DC879C63150C}">
+  <dimension ref="A1:H37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="49" customWidth="1"/>
+    <col min="5" max="5" width="49.140625" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="65">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+  </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F76DF67-2F70-4CFF-82C4-2F7D4C565685}">
+  <dimension ref="A1:H29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="49" customWidth="1"/>
+    <col min="5" max="5" width="49.140625" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" ht="260.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="262.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="49">
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="F3:F5"/>
+  </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>